<commit_message>
v0.3.0.2 alpha. RegexCheckedColumn for ListColumn is now applied per item line, not to the entire string.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20170925.xlsx
+++ b/AIWE Table Making Guideline v20170925.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common Tables" sheetId="1" r:id="rId1"/>
@@ -287,10 +287,6 @@
 &lt;reg&gt;ColumnName2=regex2&lt;/reg&gt;…&lt;reg&gt;ColumnNameN=regexN&lt;/reg&gt;</t>
   </si>
   <si>
-    <t>List of columns to be checked with regular expression. Useful for column like [Email].
-Applied only for string (nvarchar, char, varchar, etc) column.</t>
-  </si>
-  <si>
     <t>&lt;ex&gt;ColumnName1=regex1&lt;/ex&gt;
 &lt;ex&gt;ColumnName2=regex2&lt;/ex&gt;…&lt;ex&gt;ColumnNameN=regexN&lt;/ex&gt;</t>
   </si>
@@ -4141,6 +4137,55 @@
       </rPr>
       <t>,
  NullableString nvarchar(100) NULL)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of columns to be checked with regular expression. Useful for column like [Email].
+If the column checked is of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ListColumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> type, the regular expression will be applied </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>per item line</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, not the entire string
+Applied only for string (nvarchar, char, varchar, etc) column.</t>
     </r>
   </si>
 </sst>
@@ -4739,7 +4784,7 @@
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4752,7 +4797,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4765,167 +4810,167 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="35" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="35" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -4938,8 +4983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4970,7 +5015,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -5026,10 +5071,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="E6" s="32"/>
     </row>
@@ -5041,10 +5086,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="32"/>
     </row>
@@ -5053,7 +5098,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>23</v>
@@ -5068,13 +5113,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E9" s="32"/>
     </row>
@@ -5083,7 +5128,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>31</v>
@@ -5101,10 +5146,10 @@
         <v>37</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>137</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>138</v>
       </c>
       <c r="E11" s="32"/>
     </row>
@@ -5113,13 +5158,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>106</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="E12" s="32"/>
     </row>
@@ -5158,17 +5203,17 @@
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="32"/>
     </row>
-    <row r="16" spans="1:5" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>14</v>
       </c>
@@ -5178,8 +5223,8 @@
       <c r="C16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>46</v>
+      <c r="D16" s="34" t="s">
+        <v>534</v>
       </c>
       <c r="E16" s="32"/>
     </row>
@@ -5191,10 +5236,10 @@
         <v>44</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>48</v>
       </c>
       <c r="E17" s="32"/>
     </row>
@@ -5203,16 +5248,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -5241,7 +5286,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="32"/>
     </row>
@@ -5256,7 +5301,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" s="32"/>
     </row>
@@ -5271,7 +5316,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="32"/>
     </row>
@@ -5286,7 +5331,7 @@
         <v>41</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="32"/>
     </row>
@@ -5301,7 +5346,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="32"/>
     </row>
@@ -5310,16 +5355,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="E25" s="33" t="s">
         <v>325</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -5333,10 +5378,10 @@
         <v>34</v>
       </c>
       <c r="D26" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="E26" s="32" t="s">
         <v>327</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -5347,13 +5392,13 @@
         <v>18</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>329</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -5361,13 +5406,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="32"/>
     </row>
@@ -5376,13 +5421,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="32"/>
     </row>
@@ -5391,16 +5436,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>331</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="17" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
@@ -5408,16 +5453,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="E31" s="33" t="s">
         <v>333</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -5425,13 +5470,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E32" s="32"/>
     </row>
@@ -5440,13 +5485,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>182</v>
-      </c>
       <c r="D33" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E33" s="32"/>
     </row>
@@ -5455,41 +5500,41 @@
         <v>32</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D34" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>335</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5515,7 +5560,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5523,13 +5568,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -5537,13 +5582,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5551,13 +5596,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5583,23 +5628,23 @@
   <sheetData>
     <row r="1" spans="1:3" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5607,13 +5652,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5621,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5629,18 +5674,18 @@
         <v>2</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5648,18 +5693,18 @@
         <v>1</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5667,7 +5712,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5675,7 +5720,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5683,13 +5728,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5697,18 +5742,18 @@
         <v>1</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5716,7 +5761,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5724,7 +5769,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5732,7 +5777,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5740,7 +5785,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5748,7 +5793,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5756,7 +5801,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5764,18 +5809,18 @@
         <v>7</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5783,7 +5828,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5791,7 +5836,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5799,18 +5844,18 @@
         <v>3</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5818,12 +5863,12 @@
         <v>1</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5831,12 +5876,12 @@
         <v>1</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5844,12 +5889,12 @@
         <v>2</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5857,12 +5902,12 @@
         <v>3</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5870,7 +5915,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5878,7 +5923,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5886,7 +5931,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5894,7 +5939,7 @@
         <v>4</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5902,7 +5947,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5910,7 +5955,7 @@
         <v>6</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5918,7 +5963,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5926,7 +5971,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5934,7 +5979,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5942,7 +5987,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5950,18 +5995,18 @@
         <v>11</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="22" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5969,7 +6014,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5977,7 +6022,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5985,27 +6030,27 @@
         <v>3</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C68" s="22" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C69" s="22" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C70" s="22" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C71" s="22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6013,7 +6058,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6021,18 +6066,18 @@
         <v>5</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B76" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6040,12 +6085,12 @@
         <v>1</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C78" s="22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6053,17 +6098,17 @@
         <v>2</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C80" s="22" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C81" s="22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6071,22 +6116,22 @@
         <v>3</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C83" s="22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C84" s="22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B85" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6094,7 +6139,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6102,18 +6147,18 @@
         <v>2</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="89" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B90" s="22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6121,12 +6166,12 @@
         <v>1</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B92" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6134,7 +6179,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6142,7 +6187,7 @@
         <v>2</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6150,12 +6195,12 @@
         <v>3</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6163,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6171,7 +6216,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6179,28 +6224,28 @@
         <v>3</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C100" s="22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C101" s="22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B104" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6208,23 +6253,23 @@
         <v>1</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C106" s="22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="109" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B109" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="110" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6232,12 +6277,12 @@
         <v>1</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="111" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B111" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="112" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6245,17 +6290,17 @@
         <v>1</v>
       </c>
       <c r="C112" s="22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="113" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C113" s="22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="114" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B114" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="115" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6263,28 +6308,28 @@
         <v>1</v>
       </c>
       <c r="C115" s="22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="116" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C116" s="22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="117" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C117" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="119" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="120" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B120" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="121" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6292,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6300,12 +6345,12 @@
         <v>2</v>
       </c>
       <c r="C122" s="22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="123" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B123" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6313,7 +6358,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="125" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6321,7 +6366,7 @@
         <v>2</v>
       </c>
       <c r="C125" s="22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6329,18 +6374,18 @@
         <v>3</v>
       </c>
       <c r="C126" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="128" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="129" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B129" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6348,12 +6393,12 @@
         <v>1</v>
       </c>
       <c r="C130" s="22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="131" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B131" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="132" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6361,12 +6406,12 @@
         <v>1</v>
       </c>
       <c r="C132" s="22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="133" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B133" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6374,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="135" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6382,33 +6427,33 @@
         <v>2</v>
       </c>
       <c r="C135" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="136" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C136" s="22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="137" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C137" s="22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AD137" s="27"/>
     </row>
     <row r="138" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D138" s="22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="139" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D139" s="22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D140" s="26" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6416,7 +6461,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="142" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6424,7 +6469,7 @@
         <v>4</v>
       </c>
       <c r="C142" s="22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="143" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6432,12 +6477,12 @@
         <v>5</v>
       </c>
       <c r="C143" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="144" spans="2:30" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C144" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="145" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6445,18 +6490,18 @@
         <v>6</v>
       </c>
       <c r="C145" s="22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="146" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="147" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="148" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B148" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6464,7 +6509,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="150" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6472,18 +6517,18 @@
         <v>2</v>
       </c>
       <c r="C150" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="151" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="152" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="154" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6491,12 +6536,12 @@
         <v>1</v>
       </c>
       <c r="C154" s="22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="155" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B155" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6504,23 +6549,23 @@
         <v>1</v>
       </c>
       <c r="C156" s="22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="157" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C157" s="22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="158" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="159" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B160" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="161" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6528,7 +6573,7 @@
         <v>1</v>
       </c>
       <c r="C161" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="162" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6536,12 +6581,12 @@
         <v>2</v>
       </c>
       <c r="C162" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B163" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="164" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6549,7 +6594,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="165" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6557,7 +6602,7 @@
         <v>2</v>
       </c>
       <c r="C165" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6565,37 +6610,37 @@
         <v>3</v>
       </c>
       <c r="C166" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="167" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C167" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="168" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C168" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D169" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D170" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D171" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="172" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C172" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="173" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6603,18 +6648,18 @@
         <v>4</v>
       </c>
       <c r="C173" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="174" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="175" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="176" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B176" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6622,12 +6667,12 @@
         <v>1</v>
       </c>
       <c r="C177" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="178" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B178" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6635,7 +6680,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="180" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6643,7 +6688,7 @@
         <v>2</v>
       </c>
       <c r="C180" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="181" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6651,18 +6696,18 @@
         <v>3</v>
       </c>
       <c r="C181" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="182" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="183" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="184" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B184" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="185" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -6670,23 +6715,23 @@
         <v>1</v>
       </c>
       <c r="C185" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="186" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C186" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="187" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -6694,12 +6739,12 @@
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -6707,7 +6752,7 @@
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -6715,17 +6760,17 @@
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C194" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -6733,12 +6778,12 @@
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -6746,7 +6791,7 @@
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -6754,7 +6799,7 @@
         <v>2</v>
       </c>
       <c r="C199" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -6762,7 +6807,7 @@
         <v>3</v>
       </c>
       <c r="C200" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -6770,7 +6815,7 @@
         <v>4</v>
       </c>
       <c r="C201" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -6778,22 +6823,22 @@
         <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C203" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
@@ -6801,7 +6846,7 @@
         <v>1</v>
       </c>
       <c r="C207" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -6809,7 +6854,7 @@
         <v>2</v>
       </c>
       <c r="C208" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -6817,7 +6862,7 @@
         <v>3</v>
       </c>
       <c r="C209" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -6825,7 +6870,7 @@
         <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -6833,7 +6878,7 @@
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -6841,7 +6886,7 @@
         <v>6</v>
       </c>
       <c r="C212" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -6849,7 +6894,7 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -6857,7 +6902,7 @@
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -6865,17 +6910,17 @@
         <v>9</v>
       </c>
       <c r="C215" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B218" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
@@ -6883,17 +6928,17 @@
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -6901,17 +6946,17 @@
         <v>1</v>
       </c>
       <c r="C223" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B226" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
@@ -6919,7 +6964,7 @@
         <v>1</v>
       </c>
       <c r="C227" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
@@ -6927,12 +6972,12 @@
         <v>2</v>
       </c>
       <c r="C228" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -6940,27 +6985,27 @@
         <v>1</v>
       </c>
       <c r="C230" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B233" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C234" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B235" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -6968,7 +7013,7 @@
         <v>1</v>
       </c>
       <c r="C236" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
@@ -6976,7 +7021,7 @@
         <v>2</v>
       </c>
       <c r="C237" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -6984,12 +7029,12 @@
         <v>3</v>
       </c>
       <c r="C238" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B240" s="22"/>
       <c r="C240" s="22"/>
@@ -6997,7 +7042,7 @@
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="22"/>
       <c r="B241" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C241" s="22"/>
     </row>
@@ -7007,7 +7052,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
@@ -7016,13 +7061,13 @@
         <v>2</v>
       </c>
       <c r="C243" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="22"/>
       <c r="B244" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C244" s="22"/>
     </row>
@@ -7032,7 +7077,7 @@
         <v>1</v>
       </c>
       <c r="C245" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
@@ -7041,21 +7086,21 @@
         <v>2</v>
       </c>
       <c r="C246" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="22"/>
       <c r="B247" s="22"/>
       <c r="C247" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="22"/>
       <c r="B248" s="22"/>
       <c r="C248" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D248" s="22"/>
     </row>
@@ -7063,7 +7108,7 @@
       <c r="A249" s="22"/>
       <c r="B249" s="22"/>
       <c r="C249" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D249" s="22"/>
     </row>
@@ -7072,14 +7117,14 @@
       <c r="B250" s="22"/>
       <c r="C250" s="22"/>
       <c r="D250" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="22"/>
       <c r="B251" s="22"/>
       <c r="C251" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D251" s="22"/>
     </row>
@@ -7088,21 +7133,21 @@
       <c r="B252" s="22"/>
       <c r="C252" s="22"/>
       <c r="D252" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="22"/>
       <c r="B253" s="22"/>
       <c r="C253" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D253" s="22"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="22"/>
       <c r="B254" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C254" s="22"/>
       <c r="D254" s="22"/>
@@ -7113,14 +7158,14 @@
         <v>1</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D255" s="22"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="22"/>
       <c r="B256" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C256" s="22"/>
       <c r="D256" s="22"/>
@@ -7131,14 +7176,14 @@
         <v>1</v>
       </c>
       <c r="C257" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D257" s="22"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="22"/>
       <c r="B258" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C258" s="22"/>
       <c r="D258" s="22"/>
@@ -7149,18 +7194,18 @@
         <v>1</v>
       </c>
       <c r="C259" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D259" s="22"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B262" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -7168,7 +7213,7 @@
         <v>1</v>
       </c>
       <c r="C263" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -7176,7 +7221,7 @@
         <v>2</v>
       </c>
       <c r="C264" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -7184,7 +7229,7 @@
         <v>3</v>
       </c>
       <c r="C265" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -7192,12 +7237,12 @@
         <v>4</v>
       </c>
       <c r="C266" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B267" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -7205,17 +7250,17 @@
         <v>1</v>
       </c>
       <c r="C268" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C269" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C270" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -7223,12 +7268,12 @@
         <v>2</v>
       </c>
       <c r="C271" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B272" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
@@ -7236,22 +7281,22 @@
         <v>1</v>
       </c>
       <c r="C273" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C274" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C275" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C276" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
@@ -7259,12 +7304,12 @@
         <v>2</v>
       </c>
       <c r="C277" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B278" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
@@ -7272,17 +7317,17 @@
         <v>1</v>
       </c>
       <c r="C279" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B282" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
@@ -7290,7 +7335,7 @@
         <v>1</v>
       </c>
       <c r="C283" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
@@ -7298,7 +7343,7 @@
         <v>2</v>
       </c>
       <c r="C284" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
@@ -7306,7 +7351,7 @@
         <v>3</v>
       </c>
       <c r="C285" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
@@ -7314,12 +7359,12 @@
         <v>4</v>
       </c>
       <c r="C286" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
@@ -7327,22 +7372,22 @@
         <v>1</v>
       </c>
       <c r="C288" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C289" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C290" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B291" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.3">
@@ -7350,7 +7395,7 @@
         <v>1</v>
       </c>
       <c r="C292" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.3">
@@ -7358,22 +7403,22 @@
         <v>2</v>
       </c>
       <c r="C293" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C294" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C295" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B296" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
@@ -7381,17 +7426,17 @@
         <v>1</v>
       </c>
       <c r="C297" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B300" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
@@ -7399,7 +7444,7 @@
         <v>1</v>
       </c>
       <c r="C301" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -7407,7 +7452,7 @@
         <v>2</v>
       </c>
       <c r="C302" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -7415,15 +7460,15 @@
         <v>3</v>
       </c>
       <c r="C303" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B304" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D304" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
@@ -7431,28 +7476,28 @@
         <v>1</v>
       </c>
       <c r="C305" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D307" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B308" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D308" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
@@ -7460,12 +7505,12 @@
         <v>1</v>
       </c>
       <c r="C309" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B310" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -7473,17 +7518,17 @@
         <v>1</v>
       </c>
       <c r="C311" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C312" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C313" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -7491,7 +7536,7 @@
         <v>2</v>
       </c>
       <c r="C315" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
@@ -7499,12 +7544,12 @@
         <v>3</v>
       </c>
       <c r="C319" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B320" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.3">
@@ -7512,15 +7557,15 @@
         <v>1</v>
       </c>
       <c r="C321" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C322" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D322" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
@@ -7528,30 +7573,30 @@
         <v>2</v>
       </c>
       <c r="C323" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C324" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D325" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D326" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B327" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
@@ -7559,18 +7604,18 @@
         <v>1</v>
       </c>
       <c r="C328" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D328" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B329" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D329" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
@@ -7578,30 +7623,30 @@
         <v>1</v>
       </c>
       <c r="C330" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D330" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C331" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C333" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C334" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C337" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
@@ -7615,17 +7660,17 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C341" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B344" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
@@ -7633,7 +7678,7 @@
         <v>1</v>
       </c>
       <c r="C345" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
@@ -7641,17 +7686,17 @@
         <v>2</v>
       </c>
       <c r="C346" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B349" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
@@ -7659,7 +7704,7 @@
         <v>1</v>
       </c>
       <c r="C350" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
@@ -7667,12 +7712,12 @@
         <v>2</v>
       </c>
       <c r="C351" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B352" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
@@ -7680,12 +7725,12 @@
         <v>1</v>
       </c>
       <c r="C353" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B354" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
@@ -7693,17 +7738,17 @@
         <v>1</v>
       </c>
       <c r="C355" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B358" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
@@ -7711,7 +7756,7 @@
         <v>1</v>
       </c>
       <c r="C359" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
@@ -7719,7 +7764,7 @@
         <v>2</v>
       </c>
       <c r="C360" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
@@ -7727,12 +7772,12 @@
         <v>3</v>
       </c>
       <c r="C361" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B362" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
@@ -7740,7 +7785,7 @@
         <v>1</v>
       </c>
       <c r="C363" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
@@ -7748,12 +7793,12 @@
         <v>2</v>
       </c>
       <c r="C364" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C365" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
@@ -7761,17 +7806,17 @@
         <v>3</v>
       </c>
       <c r="C366" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B369" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
@@ -7779,17 +7824,17 @@
         <v>1</v>
       </c>
       <c r="C370" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B373" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -7797,7 +7842,7 @@
         <v>1</v>
       </c>
       <c r="C374" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
@@ -7805,12 +7850,12 @@
         <v>2</v>
       </c>
       <c r="C375" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B376" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -7818,7 +7863,7 @@
         <v>1</v>
       </c>
       <c r="C377" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
@@ -7826,7 +7871,7 @@
         <v>2</v>
       </c>
       <c r="C378" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -7834,7 +7879,7 @@
         <v>3</v>
       </c>
       <c r="C379" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -7842,17 +7887,17 @@
         <v>4</v>
       </c>
       <c r="C380" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B383" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
@@ -7860,12 +7905,12 @@
         <v>1</v>
       </c>
       <c r="C384" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B385" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.3">
@@ -7873,7 +7918,7 @@
         <v>1</v>
       </c>
       <c r="C386" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.3">
@@ -7881,7 +7926,7 @@
         <v>2</v>
       </c>
       <c r="C387" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.3">
@@ -7889,23 +7934,23 @@
         <v>3</v>
       </c>
       <c r="C388" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D390" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B391" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D391" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
@@ -7913,26 +7958,26 @@
         <v>1</v>
       </c>
       <c r="C392" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D392" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D394" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B395" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D395" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
@@ -7940,10 +7985,10 @@
         <v>1</v>
       </c>
       <c r="C396" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D396" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -7951,7 +7996,7 @@
         <v>2</v>
       </c>
       <c r="C397" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -7959,7 +8004,7 @@
         <v>3</v>
       </c>
       <c r="C398" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -7967,22 +8012,22 @@
         <v>4</v>
       </c>
       <c r="C399" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C400" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C401" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C402" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.3">
@@ -7990,17 +8035,17 @@
         <v>5</v>
       </c>
       <c r="C403" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B409" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.3">
@@ -8008,7 +8053,7 @@
         <v>1</v>
       </c>
       <c r="C410" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.3">
@@ -8016,15 +8061,15 @@
         <v>2</v>
       </c>
       <c r="C411" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B412" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D412" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.3">
@@ -8032,7 +8077,7 @@
         <v>1</v>
       </c>
       <c r="C413" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.3">
@@ -8040,7 +8085,7 @@
         <v>2</v>
       </c>
       <c r="C414" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.3">
@@ -8048,10 +8093,10 @@
         <v>3</v>
       </c>
       <c r="C415" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D415" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.3">
@@ -8059,20 +8104,20 @@
         <v>4</v>
       </c>
       <c r="C416" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D418" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B419" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
@@ -8080,7 +8125,7 @@
         <v>1</v>
       </c>
       <c r="C420" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.3">
@@ -8088,12 +8133,12 @@
         <v>2</v>
       </c>
       <c r="C421" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D422" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
@@ -8101,7 +8146,7 @@
         <v>3</v>
       </c>
       <c r="C423" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
@@ -8109,12 +8154,12 @@
         <v>4</v>
       </c>
       <c r="C424" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D425" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
@@ -8122,7 +8167,7 @@
         <v>5</v>
       </c>
       <c r="C426" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
@@ -8130,7 +8175,7 @@
         <v>6</v>
       </c>
       <c r="C427" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
@@ -8138,7 +8183,7 @@
         <v>7</v>
       </c>
       <c r="C429" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
@@ -8146,7 +8191,7 @@
         <v>8</v>
       </c>
       <c r="C430" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
@@ -8154,7 +8199,7 @@
         <v>9</v>
       </c>
       <c r="C431" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
@@ -8162,7 +8207,7 @@
         <v>10</v>
       </c>
       <c r="C433" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
@@ -8170,15 +8215,15 @@
         <v>11</v>
       </c>
       <c r="C434" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D434" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B436" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
@@ -8186,7 +8231,7 @@
         <v>1</v>
       </c>
       <c r="C437" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
@@ -8194,7 +8239,7 @@
         <v>2</v>
       </c>
       <c r="C438" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
@@ -8202,7 +8247,7 @@
         <v>3</v>
       </c>
       <c r="C439" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.3">
@@ -8210,7 +8255,7 @@
         <v>4</v>
       </c>
       <c r="C440" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
@@ -8218,7 +8263,7 @@
         <v>5</v>
       </c>
       <c r="C441" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
@@ -8226,7 +8271,7 @@
         <v>6</v>
       </c>
       <c r="C442" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
@@ -8234,17 +8279,17 @@
         <v>7</v>
       </c>
       <c r="C443" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B447" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -8257,7 +8302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -8271,291 +8316,291 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>381</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>383</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>384</v>
-      </c>
       <c r="C12" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="C19" s="22" t="s">
         <v>345</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>347</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>349</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>353</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>355</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>357</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>360</v>
-      </c>
       <c r="C27" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>364</v>
-      </c>
       <c r="C30" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="B35" s="22" t="s">
-        <v>370</v>
-      </c>
       <c r="C35" s="22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C39" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C40" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.4.0.0 alpha. Meta now supports ColumnSequence and ColumnAliases.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20170925.xlsx
+++ b/AIWE Table Making Guideline v20170925.xlsx
@@ -2333,7 +2333,7 @@
     <t>To give alias to the column names to appear differently from ones which appear in the table</t>
   </si>
   <si>
-    <t>To rearrange the column sequence displayed different than the sequence in the table. Not applied for Index.</t>
+    <t>To rearrange the column sequence displayed different than the sequence in the table. Not applied for Details.</t>
   </si>
 </sst>
 </file>
@@ -2556,13 +2556,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2571,6 +2569,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3145,7 +3145,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="E29" s="28"/>
     </row>
-    <row r="30" spans="1:5" s="19" customFormat="1" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" s="19" customFormat="1" ht="360" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <v>28</v>
       </c>
@@ -3674,38 +3674,38 @@
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39">
+    <row r="35" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="36">
         <v>33</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>535</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="38" t="s">
         <v>539</v>
       </c>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="1:5" s="42" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="39">
+      <c r="E35" s="39"/>
+    </row>
+    <row r="36" spans="1:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="36">
         <v>34</v>
       </c>
       <c r="B36" s="37" t="s">
         <v>536</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="38" t="s">
         <v>537</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="38" t="s">
         <v>538</v>
       </c>
-      <c r="E36" s="41"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="41" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3725,7 +3725,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="42" t="s">
         <v>313</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.4.0.1 alpha. Bug fixing for ColumnSequence and ColumnAliases.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20170925.xlsx
+++ b/AIWE Table Making Guideline v20170925.xlsx
@@ -2330,10 +2330,54 @@
     <t>To give alias to the column names to appear differently from ones which appear in the table</t>
   </si>
   <si>
-    <t>To rearrange the column sequence displayed different than the sequence in the table. Not applied for Details.</t>
-  </si>
-  <si>
     <t>ColumnName1=ColumnName1Alias;ColumnName2=ColumnName2Alias;…;ColumnNameN=ColumnNameNAlias</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To rearrange the column sequence displayed different than the sequence in the table. Only applied for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3144,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3685,7 +3729,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E35" s="39"/>
     </row>
@@ -3697,7 +3741,7 @@
         <v>536</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>537</v>

</xml_diff>

<commit_message>
v0.4.1.0 alpha. Bug fixing for ColumnSequence is now applied to all.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20170925.xlsx
+++ b/AIWE Table Making Guideline v20170925.xlsx
@@ -2327,57 +2327,17 @@
     <t>ColumnAliases</t>
   </si>
   <si>
-    <t>To give alias to the column names to appear differently from ones which appear in the table</t>
-  </si>
-  <si>
     <t>ColumnName1=ColumnName1Alias;ColumnName2=ColumnName2Alias;…;ColumnNameN=ColumnNameNAlias</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">To rearrange the column sequence displayed different than the sequence in the table. Only applied for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Create</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
+    <t>To rearrange the column sequence displayed different than the sequence in the table. 
+The rearrangement is applied to all basic actions: Index, Filter, Create, Edit, Details, and Delete.
+If only some columns are rearranged, the rearranged columns will be put first and the remaining columns are arranged with their default arrangement.
+The default arrangement is the same arrangement as the table columns arrangement.</t>
+  </si>
+  <si>
+    <t>To give alias to the column names to appear differently from ones which appear in the table.
+If alias is not specified, the default column name will be used.</t>
   </si>
 </sst>
 </file>
@@ -3718,7 +3678,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" s="40" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="36">
         <v>33</v>
       </c>
@@ -3729,7 +3689,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E35" s="39"/>
     </row>
@@ -3741,10 +3701,10 @@
         <v>536</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E36" s="39"/>
     </row>

</xml_diff>